<commit_message>
Ventajas e inconvenientes III
</commit_message>
<xml_diff>
--- a/ventajas.xlsx
+++ b/ventajas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TFG\TFG_Microservices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D524043-DC41-462A-8BAB-BEF6EB7051A3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D72DB0-09FA-4DCF-B6F0-5073E3101DB3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{C1018335-631C-40DF-AD07-76651121DFDB}"/>
   </bookViews>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="19">
   <si>
     <t>Ventaja e inconvenientes</t>
   </si>
   <si>
-    <t>Facilidad de despliegue</t>
-  </si>
-  <si>
     <t>Building microservices</t>
   </si>
   <si>
@@ -48,9 +45,6 @@
     <t>De la Torre</t>
   </si>
   <si>
-    <t>Reemplazamiento</t>
-  </si>
-  <si>
     <t>Fowler</t>
   </si>
   <si>
@@ -66,10 +60,28 @@
     <t>Consistencia eventual</t>
   </si>
   <si>
-    <t>Incremento de la deuda técnica</t>
-  </si>
-  <si>
-    <t>Microservices in production</t>
+    <t>Facilidad para evolucionar</t>
+  </si>
+  <si>
+    <t>Facilidad para ser reemplazado</t>
+  </si>
+  <si>
+    <t>Descomposición en microservicios</t>
+  </si>
+  <si>
+    <t>Integridad de los datos</t>
+  </si>
+  <si>
+    <t>Código duplicado</t>
+  </si>
+  <si>
+    <t>Advanced microservices</t>
+  </si>
+  <si>
+    <t>Alta cohesión y bajo acoplamiento</t>
+  </si>
+  <si>
+    <t>Tolerancia a fallos</t>
   </si>
 </sst>
 </file>
@@ -98,7 +110,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -106,16 +118,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD8483F6-A9E6-472D-BEB0-C27ED1F33C09}">
-  <dimension ref="B1:I12"/>
+  <dimension ref="B2:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -441,129 +472,225 @@
     <col min="1" max="1" width="3" customWidth="1"/>
     <col min="2" max="2" width="97.5546875" customWidth="1"/>
     <col min="3" max="3" width="12.5546875" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="61.8" customHeight="1">
-      <c r="B1" s="1" t="s">
+    <row r="2" spans="2:9" ht="61.8" customHeight="1">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="2:9">
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="2:9">
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="B10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="C11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="2:9">
+      <c r="B13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="B14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="B15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="2:9">
+      <c r="B16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="2:9">
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9">
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9">
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9">
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9">
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9">
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9">
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9">
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9">
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" t="s">
-        <v>3</v>
-      </c>
+      <c r="C16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>